<commit_message>
unit test for VendEmail
</commit_message>
<xml_diff>
--- a/UT.Vend.BLL/HelperFiles/tblVendContact.xlsx
+++ b/UT.Vend.BLL/HelperFiles/tblVendContact.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilson\Documents\Wilson\Documents\CISC475\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilson\Documents\Wilson\Documents\CISC475\CloneGitHub\VolTeerNET\UT.Vend.BLL\HelperFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t>Volteer.Vend.tblVendContact</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>VendorID</t>
   </si>
@@ -38,28 +35,73 @@
     <t>PrimaryContact</t>
   </si>
   <si>
-    <t>F795D2A9-245F-4F69-BE44-5C6B6F79B0C3</t>
-  </si>
-  <si>
     <t>5A41B01E-7F59-4DD2-A6C4-4CAD882BC0AB</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>6CD40064-CF05-4B55-93C0-6E4D7F9CCE34</t>
-  </si>
-  <si>
-    <t>5633998E-191B-4887-B80D-7C0357FBA367</t>
-  </si>
-  <si>
-    <t>099F7457-095D-4A38-8652-D716919622D8</t>
-  </si>
-  <si>
-    <t>F795D2A9-245F-4F69-BE44-6C5B6F79C0B3</t>
-  </si>
-  <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>FFE96E44-6447-4AB6-8EFA-0F8604D479E6</t>
+  </si>
+  <si>
+    <t>85C79F05-FF2D-46CB-8481-0FE71FD4B348</t>
+  </si>
+  <si>
+    <t>BBCF5EBB-7932-4BB0-AFAB-1445C0AEDB91</t>
+  </si>
+  <si>
+    <t>055127D5-14B1-4843-B0F9-23E451FEDC11</t>
+  </si>
+  <si>
+    <t>5C05FE31-BF50-41BB-B5B3-3B67710DEC1A</t>
+  </si>
+  <si>
+    <t>0FC01234-B8AA-4705-8FF9-4596D4AF8CFC</t>
+  </si>
+  <si>
+    <t>B6702B43-223D-48B3-88FF-6E463A521261</t>
+  </si>
+  <si>
+    <t>E4922B15-BA01-49C5-A541-A73A2EC461D9</t>
+  </si>
+  <si>
+    <t>1222663B-C1D4-4593-A288-AADC1AF70E70</t>
+  </si>
+  <si>
+    <t>6fceed59-06be-45ee-b5e6-9ee7e34ee315</t>
+  </si>
+  <si>
+    <t>861b80c6-e493-4d37-bd2a-92abc6ca4917</t>
+  </si>
+  <si>
+    <t>d4105a95-db48-4fc0-93fa-0b4099a10713</t>
+  </si>
+  <si>
+    <t>e14e476b-54a4-4edd-b922-ba243528f45e</t>
+  </si>
+  <si>
+    <t>2091e065-145a-4d94-b471-3eee9b54edbc</t>
+  </si>
+  <si>
+    <t>48f095ef-981f-4e8f-85b5-cf8d4180192a</t>
+  </si>
+  <si>
+    <t>e841c34d-7e18-4911-ab0d-6697d3268ad7</t>
+  </si>
+  <si>
+    <t>3e8b9057-a663-4214-b1b9-1ea921409a5b</t>
+  </si>
+  <si>
+    <t>0119527d-b194-445e-a676-8fd3b078d97e</t>
+  </si>
+  <si>
+    <t>055ab305-8df4-47dc-a3db-60f0cb661bcb</t>
+  </si>
+  <si>
+    <t>VolTeer.Vend.tblVendContact</t>
   </si>
 </sst>
 </file>
@@ -95,8 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,112 +422,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="164.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="164.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="str">
+        <f>"INSERT INTO " &amp; $A$2 &amp;" (" &amp; $B$1 &amp; ", " &amp; $C$1 &amp; ", " &amp; $D$1 &amp; ") VALUES('"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"' )"</f>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('6fceed59-06be-45ee-b5e6-9ee7e34ee315', 'FFE96E44-6447-4AB6-8EFA-0F8604D479E6', '1' )</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E12" si="0">"INSERT INTO " &amp; $A$2 &amp;" (" &amp; $B$1 &amp; ", " &amp; $C$1 &amp; ", " &amp; $D$1 &amp; ") VALUES('"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"' )"</f>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('861b80c6-e493-4d37-bd2a-92abc6ca4917', '85C79F05-FF2D-46CB-8481-0FE71FD4B348', '2' )</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('d4105a95-db48-4fc0-93fa-0b4099a10713', 'BBCF5EBB-7932-4BB0-AFAB-1445C0AEDB91', '3' )</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('e14e476b-54a4-4edd-b922-ba243528f45e', '055127D5-14B1-4843-B0F9-23E451FEDC11', '4' )</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('2091e065-145a-4d94-b471-3eee9b54edbc', '5C05FE31-BF50-41BB-B5B3-3B67710DEC1A', '5' )</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="str">
-        <f>"INSERT INTO " &amp; $A$1 &amp;" (" &amp; $A$2 &amp; ", " &amp; $B$2 &amp; ", " &amp; $C$2 &amp; ") VALUES("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;" )"</f>
-        <v>INSERT INTO Volteer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES(F795D2A9-245F-4F69-BE44-5C6B6F79B0C3, 5A41B01E-7F59-4DD2-A6C4-4CAD882BC0AB, 1 )</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" ref="D4:D7" si="0">"INSERT INTO " &amp; $A$1 &amp;" (" &amp; $A$2 &amp; ", " &amp; $B$2 &amp; ", " &amp; $C$2 &amp; ") VALUES("&amp;A4&amp;", "&amp;B4&amp;", "&amp;C4&amp;" )"</f>
-        <v>INSERT INTO Volteer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES(NULL, NULL, 2 )</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('48f095ef-981f-4e8f-85b5-cf8d4180192a', '0FC01234-B8AA-4705-8FF9-4596D4AF8CFC', '6' )</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('e841c34d-7e18-4911-ab0d-6697d3268ad7', '5A41B01E-7F59-4DD2-A6C4-4CAD882BC0AB', '7' )</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Volteer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES(6CD40064-CF05-4B55-93C0-6E4D7F9CCE34, 5633998E-191B-4887-B80D-7C0357FBA367, 3 )</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('3e8b9057-a663-4214-b1b9-1ea921409a5b', 'B6702B43-223D-48B3-88FF-6E463A521261', '8' )</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Volteer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES(NULL, 099F7457-095D-4A38-8652-D716919622D8, 4 )</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('0119527d-b194-445e-a676-8fd3b078d97e', 'E4922B15-BA01-49C5-A541-A73A2EC461D9', '9' )</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO Volteer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES(F795D2A9-245F-4F69-BE44-6C5B6F79C0B3, NULL, 5 )</v>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('055ab305-8df4-47dc-a3db-60f0cb661bcb', '1222663B-C1D4-4593-A288-AADC1AF70E70', '10' )</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed PrimaryContact to bool
</commit_message>
<xml_diff>
--- a/UT.Vend.BLL/HelperFiles/tblVendContact.xlsx
+++ b/UT.Vend.BLL/HelperFiles/tblVendContact.xlsx
@@ -425,7 +425,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,11 +483,11 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E12" si="0">"INSERT INTO " &amp; $A$2 &amp;" (" &amp; $B$1 &amp; ", " &amp; $C$1 &amp; ", " &amp; $D$1 &amp; ") VALUES('"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"' )"</f>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('861b80c6-e493-4d37-bd2a-92abc6ca4917', '85C79F05-FF2D-46CB-8481-0FE71FD4B348', '2' )</v>
+        <f t="shared" ref="E3:E11" si="0">"INSERT INTO " &amp; $A$2 &amp;" (" &amp; $B$1 &amp; ", " &amp; $C$1 &amp; ", " &amp; $D$1 &amp; ") VALUES('"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"' )"</f>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('861b80c6-e493-4d37-bd2a-92abc6ca4917', '85C79F05-FF2D-46CB-8481-0FE71FD4B348', '1' )</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -501,11 +501,11 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('d4105a95-db48-4fc0-93fa-0b4099a10713', 'BBCF5EBB-7932-4BB0-AFAB-1445C0AEDB91', '3' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('d4105a95-db48-4fc0-93fa-0b4099a10713', 'BBCF5EBB-7932-4BB0-AFAB-1445C0AEDB91', '1' )</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -519,11 +519,11 @@
         <v>9</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('e14e476b-54a4-4edd-b922-ba243528f45e', '055127D5-14B1-4843-B0F9-23E451FEDC11', '4' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('e14e476b-54a4-4edd-b922-ba243528f45e', '055127D5-14B1-4843-B0F9-23E451FEDC11', '1' )</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -537,11 +537,11 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('2091e065-145a-4d94-b471-3eee9b54edbc', '5C05FE31-BF50-41BB-B5B3-3B67710DEC1A', '5' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('2091e065-145a-4d94-b471-3eee9b54edbc', '5C05FE31-BF50-41BB-B5B3-3B67710DEC1A', '1' )</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -555,11 +555,11 @@
         <v>11</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('48f095ef-981f-4e8f-85b5-cf8d4180192a', '0FC01234-B8AA-4705-8FF9-4596D4AF8CFC', '6' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('48f095ef-981f-4e8f-85b5-cf8d4180192a', '0FC01234-B8AA-4705-8FF9-4596D4AF8CFC', '1' )</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -573,11 +573,11 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('e841c34d-7e18-4911-ab0d-6697d3268ad7', '5A41B01E-7F59-4DD2-A6C4-4CAD882BC0AB', '7' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('e841c34d-7e18-4911-ab0d-6697d3268ad7', '5A41B01E-7F59-4DD2-A6C4-4CAD882BC0AB', '1' )</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -591,11 +591,11 @@
         <v>12</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('3e8b9057-a663-4214-b1b9-1ea921409a5b', 'B6702B43-223D-48B3-88FF-6E463A521261', '8' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('3e8b9057-a663-4214-b1b9-1ea921409a5b', 'B6702B43-223D-48B3-88FF-6E463A521261', '1' )</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -609,11 +609,11 @@
         <v>13</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('0119527d-b194-445e-a676-8fd3b078d97e', 'E4922B15-BA01-49C5-A541-A73A2EC461D9', '9' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('0119527d-b194-445e-a676-8fd3b078d97e', 'E4922B15-BA01-49C5-A541-A73A2EC461D9', '1' )</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,11 +627,11 @@
         <v>14</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('055ab305-8df4-47dc-a3db-60f0cb661bcb', '1222663B-C1D4-4593-A288-AADC1AF70E70', '10' )</v>
+        <v>INSERT INTO VolTeer.Vend.tblVendContact (VendorID, ContactID, PrimaryContact) VALUES('055ab305-8df4-47dc-a3db-60f0cb661bcb', '1222663B-C1D4-4593-A288-AADC1AF70E70', '1' )</v>
       </c>
     </row>
   </sheetData>

</xml_diff>